<commit_message>
First attemt to set calculations for inhibition radius.
</commit_message>
<xml_diff>
--- a/www/cla/.docs/calculations.xlsx
+++ b/www/cla/.docs/calculations.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="Columns map" sheetId="1" r:id="rId1"/>
+    <sheet name="Inhibition radius" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -79,7 +80,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -100,6 +101,12 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Arabic Typesetting"/>
+      <family val="4"/>
     </font>
   </fonts>
   <fills count="7">
@@ -140,7 +147,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -148,17 +155,36 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -174,6 +200,130 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>811</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>4972</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>172528</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>188331</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="2" name="Группа 1"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="899396" y="957472"/>
+          <a:ext cx="1250019" cy="1326359"/>
+          <a:chOff x="1812131" y="1338260"/>
+          <a:chExt cx="1262063" cy="1326359"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="3" name="Прямоугольник 2"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1812131" y="1338260"/>
+            <a:ext cx="1262063" cy="1326359"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="ru-RU" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="4" name="Прямоугольник 3"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2355056" y="1907381"/>
+            <a:ext cx="180975" cy="188119"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="ru-RU" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -441,7 +591,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I321"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C179" sqref="C179"/>
     </sheetView>
@@ -658,11 +808,11 @@
         <v>314</v>
       </c>
       <c r="B8" s="3">
-        <f t="shared" ref="B8:B71" si="13">A8/16*D8</f>
+        <f t="shared" ref="B8:B17" si="13">A8/16*D8</f>
         <v>19.811612756158947</v>
       </c>
       <c r="C8" s="3">
-        <f t="shared" ref="C8:C71" si="14">A8/20*D8</f>
+        <f t="shared" ref="C8:C17" si="14">A8/20*D8</f>
         <v>15.849290204927158</v>
       </c>
       <c r="D8" s="2">
@@ -10987,11 +11137,11 @@
         <v>1</v>
       </c>
       <c r="B321" s="3">
-        <f t="shared" ref="B262:B321" si="46">A321/16*D321</f>
+        <f t="shared" ref="B321" si="46">A321/16*D321</f>
         <v>1.1180339887498949</v>
       </c>
       <c r="C321" s="3">
-        <f t="shared" ref="C262:C321" si="47">A321/20*D321</f>
+        <f t="shared" ref="C321" si="47">A321/20*D321</f>
         <v>0.89442719099991597</v>
       </c>
       <c r="D321" s="2">
@@ -11020,4 +11170,694 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="F6:V24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="265" zoomScaleNormal="265" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="2.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="16" width="2.7109375" customWidth="1"/>
+    <col min="19" max="19" width="4.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="F6" s="7">
+        <v>1</v>
+      </c>
+      <c r="G6" s="7">
+        <v>2</v>
+      </c>
+      <c r="H6" s="7">
+        <v>3</v>
+      </c>
+      <c r="I6" s="7">
+        <v>4</v>
+      </c>
+      <c r="J6" s="7">
+        <v>5</v>
+      </c>
+      <c r="K6" s="7">
+        <v>6</v>
+      </c>
+      <c r="L6" s="7">
+        <v>7</v>
+      </c>
+      <c r="M6" s="7">
+        <v>8</v>
+      </c>
+      <c r="N6" s="7">
+        <v>9</v>
+      </c>
+      <c r="O6" s="7">
+        <v>10</v>
+      </c>
+      <c r="P6" s="7">
+        <v>11</v>
+      </c>
+      <c r="Q6" s="6"/>
+      <c r="R6" s="6"/>
+      <c r="S6" s="6">
+        <v>5</v>
+      </c>
+      <c r="T6" s="6"/>
+      <c r="U6" s="6"/>
+      <c r="V6" s="6"/>
+    </row>
+    <row r="7" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="F7" s="7">
+        <v>12</v>
+      </c>
+      <c r="G7" s="7">
+        <v>13</v>
+      </c>
+      <c r="H7" s="7">
+        <v>14</v>
+      </c>
+      <c r="I7" s="7">
+        <v>15</v>
+      </c>
+      <c r="J7" s="7">
+        <v>16</v>
+      </c>
+      <c r="K7" s="7">
+        <v>17</v>
+      </c>
+      <c r="L7" s="7">
+        <v>18</v>
+      </c>
+      <c r="M7" s="7">
+        <v>19</v>
+      </c>
+      <c r="N7" s="7">
+        <v>20</v>
+      </c>
+      <c r="O7" s="7">
+        <v>21</v>
+      </c>
+      <c r="P7" s="7">
+        <v>22</v>
+      </c>
+      <c r="Q7" s="6"/>
+      <c r="R7" s="6"/>
+      <c r="S7" s="6">
+        <v>16</v>
+      </c>
+      <c r="T7" s="6"/>
+      <c r="U7" s="6"/>
+      <c r="V7" s="6"/>
+    </row>
+    <row r="8" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="F8" s="7">
+        <v>23</v>
+      </c>
+      <c r="G8" s="7">
+        <v>24</v>
+      </c>
+      <c r="H8" s="7">
+        <v>25</v>
+      </c>
+      <c r="I8" s="7">
+        <v>26</v>
+      </c>
+      <c r="J8" s="7">
+        <v>27</v>
+      </c>
+      <c r="K8" s="7">
+        <v>28</v>
+      </c>
+      <c r="L8" s="7">
+        <v>29</v>
+      </c>
+      <c r="M8" s="7">
+        <v>30</v>
+      </c>
+      <c r="N8" s="7">
+        <v>31</v>
+      </c>
+      <c r="O8" s="7">
+        <v>32</v>
+      </c>
+      <c r="P8" s="7">
+        <v>33</v>
+      </c>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="6"/>
+      <c r="S8" s="6">
+        <v>27</v>
+      </c>
+      <c r="T8" s="6"/>
+      <c r="U8" s="6"/>
+      <c r="V8" s="6"/>
+    </row>
+    <row r="9" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="F9" s="7">
+        <v>34</v>
+      </c>
+      <c r="G9" s="7">
+        <v>35</v>
+      </c>
+      <c r="H9" s="7">
+        <v>36</v>
+      </c>
+      <c r="I9" s="7">
+        <v>37</v>
+      </c>
+      <c r="J9" s="7">
+        <v>38</v>
+      </c>
+      <c r="K9" s="7">
+        <v>39</v>
+      </c>
+      <c r="L9" s="7">
+        <v>40</v>
+      </c>
+      <c r="M9" s="7">
+        <v>41</v>
+      </c>
+      <c r="N9" s="7">
+        <v>42</v>
+      </c>
+      <c r="O9" s="7">
+        <v>43</v>
+      </c>
+      <c r="P9" s="7">
+        <v>44</v>
+      </c>
+      <c r="Q9" s="6"/>
+      <c r="R9" s="6"/>
+      <c r="S9" s="6">
+        <v>38</v>
+      </c>
+      <c r="T9" s="6"/>
+      <c r="U9" s="6"/>
+      <c r="V9" s="6"/>
+    </row>
+    <row r="10" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="F10" s="7">
+        <v>45</v>
+      </c>
+      <c r="G10" s="7">
+        <v>46</v>
+      </c>
+      <c r="H10" s="7">
+        <v>47</v>
+      </c>
+      <c r="I10" s="7">
+        <v>48</v>
+      </c>
+      <c r="J10" s="7">
+        <v>49</v>
+      </c>
+      <c r="K10" s="7">
+        <v>50</v>
+      </c>
+      <c r="L10" s="7">
+        <v>51</v>
+      </c>
+      <c r="M10" s="7">
+        <v>52</v>
+      </c>
+      <c r="N10" s="7">
+        <v>53</v>
+      </c>
+      <c r="O10" s="7">
+        <v>54</v>
+      </c>
+      <c r="P10" s="7">
+        <v>55</v>
+      </c>
+      <c r="Q10" s="6"/>
+      <c r="R10" s="6"/>
+      <c r="S10" s="6">
+        <v>49</v>
+      </c>
+      <c r="T10" s="6"/>
+      <c r="U10" s="6"/>
+      <c r="V10" s="6"/>
+    </row>
+    <row r="11" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="F11" s="7">
+        <v>56</v>
+      </c>
+      <c r="G11" s="7">
+        <v>57</v>
+      </c>
+      <c r="H11" s="7">
+        <v>58</v>
+      </c>
+      <c r="I11" s="7">
+        <v>59</v>
+      </c>
+      <c r="J11" s="7">
+        <v>60</v>
+      </c>
+      <c r="K11" s="7">
+        <v>61</v>
+      </c>
+      <c r="L11" s="7">
+        <v>62</v>
+      </c>
+      <c r="M11" s="7">
+        <v>63</v>
+      </c>
+      <c r="N11" s="7">
+        <v>64</v>
+      </c>
+      <c r="O11" s="7">
+        <v>65</v>
+      </c>
+      <c r="P11" s="7">
+        <v>66</v>
+      </c>
+      <c r="Q11" s="6"/>
+      <c r="R11" s="6"/>
+      <c r="S11" s="6">
+        <v>60</v>
+      </c>
+      <c r="T11" s="6"/>
+      <c r="U11" s="6"/>
+      <c r="V11" s="6"/>
+    </row>
+    <row r="12" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="F12" s="7">
+        <v>67</v>
+      </c>
+      <c r="G12" s="7">
+        <v>68</v>
+      </c>
+      <c r="H12" s="7">
+        <v>69</v>
+      </c>
+      <c r="I12" s="7">
+        <v>70</v>
+      </c>
+      <c r="J12" s="7">
+        <v>71</v>
+      </c>
+      <c r="K12" s="7">
+        <v>72</v>
+      </c>
+      <c r="L12" s="7">
+        <v>73</v>
+      </c>
+      <c r="M12" s="7">
+        <v>74</v>
+      </c>
+      <c r="N12" s="7">
+        <v>75</v>
+      </c>
+      <c r="O12" s="7">
+        <v>76</v>
+      </c>
+      <c r="P12" s="7">
+        <v>77</v>
+      </c>
+      <c r="Q12" s="6"/>
+      <c r="R12" s="6"/>
+      <c r="S12" s="6">
+        <v>71</v>
+      </c>
+      <c r="T12" s="6"/>
+      <c r="U12" s="6"/>
+      <c r="V12" s="6"/>
+    </row>
+    <row r="13" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="F13" s="7">
+        <v>78</v>
+      </c>
+      <c r="G13" s="7">
+        <v>79</v>
+      </c>
+      <c r="H13" s="7">
+        <v>80</v>
+      </c>
+      <c r="I13" s="7">
+        <v>81</v>
+      </c>
+      <c r="J13" s="7">
+        <v>82</v>
+      </c>
+      <c r="K13" s="7">
+        <v>83</v>
+      </c>
+      <c r="L13" s="7">
+        <v>84</v>
+      </c>
+      <c r="M13" s="7">
+        <v>85</v>
+      </c>
+      <c r="N13" s="7">
+        <v>86</v>
+      </c>
+      <c r="O13" s="7">
+        <v>87</v>
+      </c>
+      <c r="P13" s="7">
+        <v>88</v>
+      </c>
+      <c r="Q13" s="6"/>
+      <c r="R13" s="6"/>
+      <c r="S13" s="6">
+        <v>82</v>
+      </c>
+      <c r="T13" s="6"/>
+      <c r="U13" s="6"/>
+      <c r="V13" s="6"/>
+    </row>
+    <row r="14" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="F14" s="7">
+        <v>89</v>
+      </c>
+      <c r="G14" s="7">
+        <v>90</v>
+      </c>
+      <c r="H14" s="7">
+        <v>91</v>
+      </c>
+      <c r="I14" s="7">
+        <v>92</v>
+      </c>
+      <c r="J14" s="7">
+        <v>93</v>
+      </c>
+      <c r="K14" s="7">
+        <v>94</v>
+      </c>
+      <c r="L14" s="7">
+        <v>95</v>
+      </c>
+      <c r="M14" s="7">
+        <v>96</v>
+      </c>
+      <c r="N14" s="7">
+        <v>97</v>
+      </c>
+      <c r="O14" s="7">
+        <v>98</v>
+      </c>
+      <c r="P14" s="7">
+        <v>99</v>
+      </c>
+      <c r="Q14" s="6"/>
+      <c r="R14" s="6"/>
+      <c r="S14" s="6">
+        <v>93</v>
+      </c>
+      <c r="T14" s="6"/>
+      <c r="U14" s="6"/>
+      <c r="V14" s="6"/>
+    </row>
+    <row r="15" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="F15" s="7">
+        <v>100</v>
+      </c>
+      <c r="G15" s="7">
+        <v>101</v>
+      </c>
+      <c r="H15" s="7">
+        <v>102</v>
+      </c>
+      <c r="I15" s="7">
+        <v>103</v>
+      </c>
+      <c r="J15" s="7">
+        <v>104</v>
+      </c>
+      <c r="K15" s="7">
+        <v>105</v>
+      </c>
+      <c r="L15" s="7">
+        <v>106</v>
+      </c>
+      <c r="M15" s="7">
+        <v>107</v>
+      </c>
+      <c r="N15" s="7">
+        <v>108</v>
+      </c>
+      <c r="O15" s="7">
+        <v>109</v>
+      </c>
+      <c r="P15" s="7">
+        <v>110</v>
+      </c>
+      <c r="Q15" s="6"/>
+      <c r="R15" s="6"/>
+      <c r="S15" s="6">
+        <v>104</v>
+      </c>
+      <c r="T15" s="6"/>
+      <c r="U15" s="6"/>
+      <c r="V15" s="6"/>
+    </row>
+    <row r="16" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="F16" s="7">
+        <v>111</v>
+      </c>
+      <c r="G16" s="7">
+        <v>112</v>
+      </c>
+      <c r="H16" s="7">
+        <v>113</v>
+      </c>
+      <c r="I16" s="7">
+        <v>114</v>
+      </c>
+      <c r="J16" s="7">
+        <v>115</v>
+      </c>
+      <c r="K16" s="7">
+        <v>116</v>
+      </c>
+      <c r="L16" s="7">
+        <v>117</v>
+      </c>
+      <c r="M16" s="7">
+        <v>118</v>
+      </c>
+      <c r="N16" s="7">
+        <v>119</v>
+      </c>
+      <c r="O16" s="7">
+        <v>120</v>
+      </c>
+      <c r="P16" s="7">
+        <v>121</v>
+      </c>
+      <c r="Q16" s="6"/>
+      <c r="R16" s="6"/>
+      <c r="S16" s="6">
+        <v>115</v>
+      </c>
+      <c r="T16" s="6"/>
+      <c r="U16" s="6"/>
+      <c r="V16" s="6"/>
+    </row>
+    <row r="17" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="F17" s="7">
+        <v>122</v>
+      </c>
+      <c r="G17" s="7">
+        <v>123</v>
+      </c>
+      <c r="H17" s="7">
+        <v>124</v>
+      </c>
+      <c r="I17" s="7">
+        <v>125</v>
+      </c>
+      <c r="J17" s="7">
+        <v>126</v>
+      </c>
+      <c r="K17" s="7">
+        <v>127</v>
+      </c>
+      <c r="L17" s="7">
+        <v>128</v>
+      </c>
+      <c r="M17" s="7">
+        <v>129</v>
+      </c>
+      <c r="N17" s="7">
+        <v>130</v>
+      </c>
+      <c r="O17" s="7">
+        <v>131</v>
+      </c>
+      <c r="P17" s="7">
+        <v>132</v>
+      </c>
+      <c r="Q17" s="6"/>
+      <c r="R17" s="6"/>
+      <c r="S17" s="6"/>
+      <c r="T17" s="6"/>
+      <c r="U17" s="6"/>
+      <c r="V17" s="6"/>
+    </row>
+    <row r="18" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="F18" s="7">
+        <v>133</v>
+      </c>
+      <c r="G18" s="7">
+        <v>134</v>
+      </c>
+      <c r="H18" s="7">
+        <v>135</v>
+      </c>
+      <c r="I18" s="7">
+        <v>136</v>
+      </c>
+      <c r="J18" s="7">
+        <v>137</v>
+      </c>
+      <c r="K18" s="7">
+        <v>138</v>
+      </c>
+      <c r="L18" s="7">
+        <v>139</v>
+      </c>
+      <c r="M18" s="7">
+        <v>140</v>
+      </c>
+      <c r="N18" s="7">
+        <v>141</v>
+      </c>
+      <c r="O18" s="7">
+        <v>142</v>
+      </c>
+      <c r="P18" s="7">
+        <v>143</v>
+      </c>
+      <c r="Q18" s="6"/>
+      <c r="R18" s="6"/>
+      <c r="S18" s="6"/>
+      <c r="T18" s="6"/>
+      <c r="U18" s="6"/>
+      <c r="V18" s="6"/>
+    </row>
+    <row r="19" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="6"/>
+      <c r="L19" s="6"/>
+      <c r="M19" s="6"/>
+      <c r="N19" s="6"/>
+      <c r="O19" s="6"/>
+      <c r="P19" s="6"/>
+      <c r="Q19" s="6"/>
+      <c r="R19" s="6"/>
+      <c r="S19" s="6"/>
+      <c r="T19" s="6"/>
+      <c r="U19" s="6"/>
+      <c r="V19" s="6"/>
+    </row>
+    <row r="20" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="6"/>
+      <c r="M20" s="6"/>
+      <c r="N20" s="6"/>
+      <c r="O20" s="6"/>
+      <c r="P20" s="6"/>
+      <c r="Q20" s="6"/>
+      <c r="R20" s="6"/>
+      <c r="S20" s="6"/>
+      <c r="T20" s="6"/>
+      <c r="U20" s="6"/>
+      <c r="V20" s="6"/>
+    </row>
+    <row r="21" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
+      <c r="L21" s="6"/>
+      <c r="M21" s="6"/>
+      <c r="N21" s="6"/>
+      <c r="O21" s="6"/>
+      <c r="P21" s="6"/>
+      <c r="Q21" s="6"/>
+      <c r="R21" s="6"/>
+      <c r="S21" s="6"/>
+      <c r="T21" s="6"/>
+      <c r="U21" s="6"/>
+      <c r="V21" s="6"/>
+    </row>
+    <row r="22" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="6"/>
+      <c r="L22" s="6"/>
+      <c r="M22" s="6"/>
+      <c r="N22" s="6"/>
+      <c r="O22" s="6"/>
+      <c r="P22" s="6"/>
+      <c r="Q22" s="6"/>
+      <c r="R22" s="6"/>
+      <c r="S22" s="6"/>
+      <c r="T22" s="6"/>
+      <c r="U22" s="6"/>
+      <c r="V22" s="6"/>
+    </row>
+    <row r="23" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="6"/>
+      <c r="L23" s="6"/>
+      <c r="M23" s="6"/>
+      <c r="N23" s="6"/>
+      <c r="O23" s="6"/>
+      <c r="P23" s="6"/>
+      <c r="Q23" s="6"/>
+      <c r="R23" s="6"/>
+      <c r="S23" s="6"/>
+      <c r="T23" s="6"/>
+      <c r="U23" s="6"/>
+      <c r="V23" s="6"/>
+    </row>
+    <row r="24" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="6"/>
+      <c r="L24" s="6"/>
+      <c r="M24" s="6"/>
+      <c r="N24" s="6"/>
+      <c r="O24" s="6"/>
+      <c r="P24" s="6"/>
+      <c r="Q24" s="6"/>
+      <c r="R24" s="6"/>
+      <c r="S24" s="6"/>
+      <c r="T24" s="6"/>
+      <c r="U24" s="6"/>
+      <c r="V24" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
setInhibitionRadius - now is as a function. Some improvement remains.
</commit_message>
<xml_diff>
--- a/www/cla/.docs/calculations.xlsx
+++ b/www/cla/.docs/calculations.xlsx
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
     <t>Коэффициент</t>
   </si>
@@ -75,12 +75,24 @@
   <si>
     <t>Кв. корень</t>
   </si>
+  <si>
+    <t>3-2</t>
+  </si>
+  <si>
+    <t>0,-1,-2</t>
+  </si>
+  <si>
+    <t>-1</t>
+  </si>
+  <si>
+    <t>=4+11-7+3</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -107,6 +119,14 @@
       <color theme="1"/>
       <name val="Arabic Typesetting"/>
       <family val="4"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="7">
@@ -174,7 +194,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -185,6 +205,11 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -206,16 +231,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>811</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>4972</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>4688</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>185533</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>172528</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>177895</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>188331</xdr:rowOff>
+      <xdr:rowOff>178392</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
@@ -224,8 +249,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="899396" y="957472"/>
-          <a:ext cx="1250019" cy="1326359"/>
+          <a:off x="548310" y="947533"/>
+          <a:ext cx="1260451" cy="1326359"/>
           <a:chOff x="1812131" y="1338260"/>
           <a:chExt cx="1262063" cy="1326359"/>
         </a:xfrm>
@@ -11174,585 +11199,648 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="F6:V24"/>
+  <dimension ref="F5:X26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="265" zoomScaleNormal="265" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="U9" sqref="U9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="6" max="16" width="2.7109375" customWidth="1"/>
     <col min="19" max="19" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="6:22" x14ac:dyDescent="0.25">
-      <c r="F6" s="7">
+    <row r="5" spans="6:24" x14ac:dyDescent="0.25">
+      <c r="U5" s="10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="6:24" x14ac:dyDescent="0.25">
+      <c r="F6" s="8">
+        <v>-22</v>
+      </c>
+      <c r="G6" s="8">
+        <v>-21</v>
+      </c>
+      <c r="H6" s="8">
+        <v>-20</v>
+      </c>
+      <c r="I6" s="8">
+        <v>-19</v>
+      </c>
+      <c r="J6" s="8">
+        <v>-18</v>
+      </c>
+      <c r="K6" s="8">
+        <v>-17</v>
+      </c>
+      <c r="L6" s="8">
+        <v>-16</v>
+      </c>
+      <c r="M6" s="8">
+        <v>-15</v>
+      </c>
+      <c r="N6" s="8">
+        <v>-14</v>
+      </c>
+      <c r="O6" s="8">
+        <v>-13</v>
+      </c>
+      <c r="P6" s="8">
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="7" spans="6:24" x14ac:dyDescent="0.25">
+      <c r="F7" s="8">
+        <v>-11</v>
+      </c>
+      <c r="G7" s="8">
+        <v>-10</v>
+      </c>
+      <c r="H7" s="8">
+        <v>-9</v>
+      </c>
+      <c r="I7" s="8">
+        <v>-8</v>
+      </c>
+      <c r="J7" s="8">
+        <v>-7</v>
+      </c>
+      <c r="K7" s="8">
+        <v>-6</v>
+      </c>
+      <c r="L7" s="8">
+        <v>-5</v>
+      </c>
+      <c r="M7" s="8">
+        <v>-4</v>
+      </c>
+      <c r="N7" s="8">
+        <v>-3</v>
+      </c>
+      <c r="O7" s="8">
+        <v>-2</v>
+      </c>
+      <c r="P7" s="8">
+        <v>-1</v>
+      </c>
+      <c r="Q7" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="6:24" x14ac:dyDescent="0.25">
+      <c r="F8" s="7">
         <v>1</v>
       </c>
-      <c r="G6" s="7">
+      <c r="G8" s="7">
         <v>2</v>
       </c>
-      <c r="H6" s="7">
+      <c r="H8" s="7">
         <v>3</v>
       </c>
-      <c r="I6" s="7">
+      <c r="I8" s="7">
         <v>4</v>
       </c>
-      <c r="J6" s="7">
+      <c r="J8" s="7">
         <v>5</v>
       </c>
-      <c r="K6" s="7">
+      <c r="K8" s="7">
         <v>6</v>
       </c>
-      <c r="L6" s="7">
+      <c r="L8" s="7">
         <v>7</v>
       </c>
-      <c r="M6" s="7">
+      <c r="M8" s="7">
         <v>8</v>
       </c>
-      <c r="N6" s="7">
+      <c r="N8" s="7">
         <v>9</v>
       </c>
-      <c r="O6" s="7">
+      <c r="O8" s="7">
         <v>10</v>
       </c>
-      <c r="P6" s="7">
+      <c r="P8" s="7">
         <v>11</v>
-      </c>
-      <c r="Q6" s="6"/>
-      <c r="R6" s="6"/>
-      <c r="S6" s="6">
-        <v>5</v>
-      </c>
-      <c r="T6" s="6"/>
-      <c r="U6" s="6"/>
-      <c r="V6" s="6"/>
-    </row>
-    <row r="7" spans="6:22" x14ac:dyDescent="0.25">
-      <c r="F7" s="7">
-        <v>12</v>
-      </c>
-      <c r="G7" s="7">
-        <v>13</v>
-      </c>
-      <c r="H7" s="7">
-        <v>14</v>
-      </c>
-      <c r="I7" s="7">
-        <v>15</v>
-      </c>
-      <c r="J7" s="7">
-        <v>16</v>
-      </c>
-      <c r="K7" s="7">
-        <v>17</v>
-      </c>
-      <c r="L7" s="7">
-        <v>18</v>
-      </c>
-      <c r="M7" s="7">
-        <v>19</v>
-      </c>
-      <c r="N7" s="7">
-        <v>20</v>
-      </c>
-      <c r="O7" s="7">
-        <v>21</v>
-      </c>
-      <c r="P7" s="7">
-        <v>22</v>
-      </c>
-      <c r="Q7" s="6"/>
-      <c r="R7" s="6"/>
-      <c r="S7" s="6">
-        <v>16</v>
-      </c>
-      <c r="T7" s="6"/>
-      <c r="U7" s="6"/>
-      <c r="V7" s="6"/>
-    </row>
-    <row r="8" spans="6:22" x14ac:dyDescent="0.25">
-      <c r="F8" s="7">
-        <v>23</v>
-      </c>
-      <c r="G8" s="7">
-        <v>24</v>
-      </c>
-      <c r="H8" s="7">
-        <v>25</v>
-      </c>
-      <c r="I8" s="7">
-        <v>26</v>
-      </c>
-      <c r="J8" s="7">
-        <v>27</v>
-      </c>
-      <c r="K8" s="7">
-        <v>28</v>
-      </c>
-      <c r="L8" s="7">
-        <v>29</v>
-      </c>
-      <c r="M8" s="7">
-        <v>30</v>
-      </c>
-      <c r="N8" s="7">
-        <v>31</v>
-      </c>
-      <c r="O8" s="7">
-        <v>32</v>
-      </c>
-      <c r="P8" s="7">
-        <v>33</v>
       </c>
       <c r="Q8" s="6"/>
       <c r="R8" s="6"/>
       <c r="S8" s="6">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="T8" s="6"/>
-      <c r="U8" s="6"/>
+      <c r="U8" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="V8" s="6"/>
     </row>
-    <row r="9" spans="6:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F9" s="7">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="G9" s="7">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="H9" s="7">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="I9" s="7">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="J9" s="7">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="K9" s="7">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="L9" s="7">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="M9" s="7">
-        <v>41</v>
+        <v>19</v>
       </c>
       <c r="N9" s="7">
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="O9" s="7">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="P9" s="7">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="Q9" s="6"/>
       <c r="R9" s="6"/>
       <c r="S9" s="6">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="T9" s="6"/>
       <c r="U9" s="6"/>
       <c r="V9" s="6"/>
     </row>
-    <row r="10" spans="6:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F10" s="7">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="G10" s="7">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="H10" s="7">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="I10" s="7">
-        <v>48</v>
+        <v>26</v>
       </c>
       <c r="J10" s="7">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="K10" s="7">
-        <v>50</v>
+        <v>28</v>
       </c>
       <c r="L10" s="7">
-        <v>51</v>
+        <v>29</v>
       </c>
       <c r="M10" s="7">
-        <v>52</v>
+        <v>30</v>
       </c>
       <c r="N10" s="7">
-        <v>53</v>
+        <v>31</v>
       </c>
       <c r="O10" s="7">
-        <v>54</v>
+        <v>32</v>
       </c>
       <c r="P10" s="7">
-        <v>55</v>
+        <v>33</v>
       </c>
       <c r="Q10" s="6"/>
       <c r="R10" s="6"/>
       <c r="S10" s="6">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="T10" s="6"/>
       <c r="U10" s="6"/>
       <c r="V10" s="6"/>
     </row>
-    <row r="11" spans="6:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F11" s="7">
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="G11" s="7">
-        <v>57</v>
+        <v>35</v>
       </c>
       <c r="H11" s="7">
-        <v>58</v>
+        <v>36</v>
       </c>
       <c r="I11" s="7">
-        <v>59</v>
+        <v>37</v>
       </c>
       <c r="J11" s="7">
-        <v>60</v>
+        <v>38</v>
       </c>
       <c r="K11" s="7">
-        <v>61</v>
+        <v>39</v>
       </c>
       <c r="L11" s="7">
-        <v>62</v>
+        <v>40</v>
       </c>
       <c r="M11" s="7">
-        <v>63</v>
+        <v>41</v>
       </c>
       <c r="N11" s="7">
-        <v>64</v>
+        <v>42</v>
       </c>
       <c r="O11" s="7">
-        <v>65</v>
+        <v>43</v>
       </c>
       <c r="P11" s="7">
-        <v>66</v>
+        <v>44</v>
       </c>
       <c r="Q11" s="6"/>
       <c r="R11" s="6"/>
       <c r="S11" s="6">
-        <v>60</v>
+        <v>38</v>
       </c>
       <c r="T11" s="6"/>
-      <c r="U11" s="6"/>
-      <c r="V11" s="6"/>
-    </row>
-    <row r="12" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="U11" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="V11" s="6">
+        <v>0</v>
+      </c>
+      <c r="W11">
+        <v>-1</v>
+      </c>
+      <c r="X11">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="12" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F12" s="7">
-        <v>67</v>
+        <v>45</v>
       </c>
       <c r="G12" s="7">
-        <v>68</v>
+        <v>46</v>
       </c>
       <c r="H12" s="7">
-        <v>69</v>
+        <v>47</v>
       </c>
       <c r="I12" s="7">
-        <v>70</v>
+        <v>48</v>
       </c>
       <c r="J12" s="7">
-        <v>71</v>
+        <v>49</v>
       </c>
       <c r="K12" s="7">
-        <v>72</v>
+        <v>50</v>
       </c>
       <c r="L12" s="7">
-        <v>73</v>
+        <v>51</v>
       </c>
       <c r="M12" s="7">
-        <v>74</v>
+        <v>52</v>
       </c>
       <c r="N12" s="7">
-        <v>75</v>
+        <v>53</v>
       </c>
       <c r="O12" s="7">
-        <v>76</v>
+        <v>54</v>
       </c>
       <c r="P12" s="7">
-        <v>77</v>
+        <v>55</v>
       </c>
       <c r="Q12" s="6"/>
       <c r="R12" s="6"/>
       <c r="S12" s="6">
-        <v>71</v>
+        <v>49</v>
       </c>
       <c r="T12" s="6"/>
       <c r="U12" s="6"/>
-      <c r="V12" s="6"/>
-    </row>
-    <row r="13" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="V12" s="6">
+        <v>1</v>
+      </c>
+      <c r="W12">
+        <v>2</v>
+      </c>
+      <c r="X12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F13" s="7">
-        <v>78</v>
+        <v>56</v>
       </c>
       <c r="G13" s="7">
-        <v>79</v>
+        <v>57</v>
       </c>
       <c r="H13" s="7">
-        <v>80</v>
+        <v>58</v>
       </c>
       <c r="I13" s="7">
-        <v>81</v>
+        <v>59</v>
       </c>
       <c r="J13" s="7">
-        <v>82</v>
+        <v>60</v>
       </c>
       <c r="K13" s="7">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="L13" s="7">
-        <v>84</v>
+        <v>62</v>
       </c>
       <c r="M13" s="7">
-        <v>85</v>
+        <v>63</v>
       </c>
       <c r="N13" s="7">
-        <v>86</v>
+        <v>64</v>
       </c>
       <c r="O13" s="7">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="P13" s="7">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="Q13" s="6"/>
       <c r="R13" s="6"/>
       <c r="S13" s="6">
-        <v>82</v>
+        <v>60</v>
       </c>
       <c r="T13" s="6"/>
       <c r="U13" s="6"/>
       <c r="V13" s="6"/>
     </row>
-    <row r="14" spans="6:22" x14ac:dyDescent="0.25">
+    <row r="14" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F14" s="7">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="G14" s="7">
-        <v>90</v>
+        <v>68</v>
       </c>
       <c r="H14" s="7">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="I14" s="7">
-        <v>92</v>
+        <v>70</v>
       </c>
       <c r="J14" s="7">
-        <v>93</v>
+        <v>71</v>
       </c>
       <c r="K14" s="7">
-        <v>94</v>
+        <v>72</v>
       </c>
       <c r="L14" s="7">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="M14" s="7">
-        <v>96</v>
+        <v>74</v>
       </c>
       <c r="N14" s="7">
-        <v>97</v>
+        <v>75</v>
       </c>
       <c r="O14" s="7">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="P14" s="7">
-        <v>99</v>
+        <v>77</v>
       </c>
       <c r="Q14" s="6"/>
       <c r="R14" s="6"/>
       <c r="S14" s="6">
-        <v>93</v>
+        <v>71</v>
       </c>
       <c r="T14" s="6"/>
       <c r="U14" s="6"/>
       <c r="V14" s="6"/>
     </row>
-    <row r="15" spans="6:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F15" s="7">
-        <v>100</v>
+        <v>78</v>
       </c>
       <c r="G15" s="7">
-        <v>101</v>
+        <v>79</v>
       </c>
       <c r="H15" s="7">
-        <v>102</v>
+        <v>80</v>
       </c>
       <c r="I15" s="7">
-        <v>103</v>
+        <v>81</v>
       </c>
       <c r="J15" s="7">
-        <v>104</v>
+        <v>82</v>
       </c>
       <c r="K15" s="7">
-        <v>105</v>
+        <v>83</v>
       </c>
       <c r="L15" s="7">
-        <v>106</v>
+        <v>84</v>
       </c>
       <c r="M15" s="7">
-        <v>107</v>
+        <v>85</v>
       </c>
       <c r="N15" s="7">
-        <v>108</v>
+        <v>86</v>
       </c>
       <c r="O15" s="7">
-        <v>109</v>
+        <v>87</v>
       </c>
       <c r="P15" s="7">
-        <v>110</v>
+        <v>88</v>
       </c>
       <c r="Q15" s="6"/>
       <c r="R15" s="6"/>
       <c r="S15" s="6">
-        <v>104</v>
+        <v>82</v>
       </c>
       <c r="T15" s="6"/>
       <c r="U15" s="6"/>
-      <c r="V15" s="6"/>
-    </row>
-    <row r="16" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="V15" s="6">
+        <v>1</v>
+      </c>
+      <c r="W15" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="X15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F16" s="7">
-        <v>111</v>
+        <v>89</v>
       </c>
       <c r="G16" s="7">
-        <v>112</v>
+        <v>90</v>
       </c>
       <c r="H16" s="7">
-        <v>113</v>
+        <v>91</v>
       </c>
       <c r="I16" s="7">
-        <v>114</v>
+        <v>92</v>
       </c>
       <c r="J16" s="7">
-        <v>115</v>
+        <v>93</v>
       </c>
       <c r="K16" s="7">
-        <v>116</v>
+        <v>94</v>
       </c>
       <c r="L16" s="7">
-        <v>117</v>
+        <v>95</v>
       </c>
       <c r="M16" s="7">
-        <v>118</v>
+        <v>96</v>
       </c>
       <c r="N16" s="7">
-        <v>119</v>
+        <v>97</v>
       </c>
       <c r="O16" s="7">
-        <v>120</v>
+        <v>98</v>
       </c>
       <c r="P16" s="7">
-        <v>121</v>
+        <v>99</v>
       </c>
       <c r="Q16" s="6"/>
       <c r="R16" s="6"/>
       <c r="S16" s="6">
-        <v>115</v>
+        <v>93</v>
       </c>
       <c r="T16" s="6"/>
       <c r="U16" s="6"/>
-      <c r="V16" s="6"/>
-    </row>
-    <row r="17" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="V16" s="11">
+        <v>2</v>
+      </c>
+      <c r="W16" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="X16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F17" s="7">
-        <v>122</v>
+        <v>100</v>
       </c>
       <c r="G17" s="7">
-        <v>123</v>
+        <v>101</v>
       </c>
       <c r="H17" s="7">
-        <v>124</v>
+        <v>102</v>
       </c>
       <c r="I17" s="7">
-        <v>125</v>
+        <v>103</v>
       </c>
       <c r="J17" s="7">
-        <v>126</v>
+        <v>104</v>
       </c>
       <c r="K17" s="7">
-        <v>127</v>
+        <v>105</v>
       </c>
       <c r="L17" s="7">
-        <v>128</v>
+        <v>106</v>
       </c>
       <c r="M17" s="7">
-        <v>129</v>
+        <v>107</v>
       </c>
       <c r="N17" s="7">
-        <v>130</v>
+        <v>108</v>
       </c>
       <c r="O17" s="7">
-        <v>131</v>
+        <v>109</v>
       </c>
       <c r="P17" s="7">
-        <v>132</v>
+        <v>110</v>
       </c>
       <c r="Q17" s="6"/>
       <c r="R17" s="6"/>
-      <c r="S17" s="6"/>
+      <c r="S17" s="6">
+        <v>104</v>
+      </c>
       <c r="T17" s="6"/>
       <c r="U17" s="6"/>
-      <c r="V17" s="6"/>
-    </row>
-    <row r="18" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="V17" s="11">
+        <v>3</v>
+      </c>
+      <c r="W17" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="X17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F18" s="7">
-        <v>133</v>
+        <v>111</v>
       </c>
       <c r="G18" s="7">
-        <v>134</v>
+        <v>112</v>
       </c>
       <c r="H18" s="7">
-        <v>135</v>
+        <v>113</v>
       </c>
       <c r="I18" s="7">
-        <v>136</v>
+        <v>114</v>
       </c>
       <c r="J18" s="7">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="K18" s="7">
-        <v>138</v>
+        <v>116</v>
       </c>
       <c r="L18" s="7">
-        <v>139</v>
+        <v>117</v>
       </c>
       <c r="M18" s="7">
-        <v>140</v>
+        <v>118</v>
       </c>
       <c r="N18" s="7">
-        <v>141</v>
+        <v>119</v>
       </c>
       <c r="O18" s="7">
-        <v>142</v>
+        <v>120</v>
       </c>
       <c r="P18" s="7">
-        <v>143</v>
+        <v>121</v>
       </c>
       <c r="Q18" s="6"/>
       <c r="R18" s="6"/>
-      <c r="S18" s="6"/>
+      <c r="S18" s="6">
+        <v>115</v>
+      </c>
       <c r="T18" s="6"/>
       <c r="U18" s="6"/>
       <c r="V18" s="6"/>
     </row>
-    <row r="19" spans="6:22" x14ac:dyDescent="0.25">
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="6"/>
-      <c r="L19" s="6"/>
-      <c r="M19" s="6"/>
-      <c r="N19" s="6"/>
-      <c r="O19" s="6"/>
-      <c r="P19" s="6"/>
+    <row r="19" spans="6:24" x14ac:dyDescent="0.25">
+      <c r="F19" s="7">
+        <v>122</v>
+      </c>
+      <c r="G19" s="7">
+        <v>123</v>
+      </c>
+      <c r="H19" s="7">
+        <v>124</v>
+      </c>
+      <c r="I19" s="7">
+        <v>125</v>
+      </c>
+      <c r="J19" s="7">
+        <v>126</v>
+      </c>
+      <c r="K19" s="7">
+        <v>127</v>
+      </c>
+      <c r="L19" s="7">
+        <v>128</v>
+      </c>
+      <c r="M19" s="7">
+        <v>129</v>
+      </c>
+      <c r="N19" s="7">
+        <v>130</v>
+      </c>
+      <c r="O19" s="7">
+        <v>131</v>
+      </c>
+      <c r="P19" s="7">
+        <v>132</v>
+      </c>
       <c r="Q19" s="6"/>
       <c r="R19" s="6"/>
       <c r="S19" s="6"/>
@@ -11760,18 +11848,40 @@
       <c r="U19" s="6"/>
       <c r="V19" s="6"/>
     </row>
-    <row r="20" spans="6:22" x14ac:dyDescent="0.25">
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="6"/>
-      <c r="K20" s="6"/>
-      <c r="L20" s="6"/>
-      <c r="M20" s="6"/>
-      <c r="N20" s="6"/>
-      <c r="O20" s="6"/>
-      <c r="P20" s="6"/>
+    <row r="20" spans="6:24" x14ac:dyDescent="0.25">
+      <c r="F20" s="7">
+        <v>133</v>
+      </c>
+      <c r="G20" s="7">
+        <v>134</v>
+      </c>
+      <c r="H20" s="7">
+        <v>135</v>
+      </c>
+      <c r="I20" s="7">
+        <v>136</v>
+      </c>
+      <c r="J20" s="7">
+        <v>137</v>
+      </c>
+      <c r="K20" s="7">
+        <v>138</v>
+      </c>
+      <c r="L20" s="7">
+        <v>139</v>
+      </c>
+      <c r="M20" s="7">
+        <v>140</v>
+      </c>
+      <c r="N20" s="7">
+        <v>141</v>
+      </c>
+      <c r="O20" s="7">
+        <v>142</v>
+      </c>
+      <c r="P20" s="7">
+        <v>143</v>
+      </c>
       <c r="Q20" s="6"/>
       <c r="R20" s="6"/>
       <c r="S20" s="6"/>
@@ -11779,7 +11889,7 @@
       <c r="U20" s="6"/>
       <c r="V20" s="6"/>
     </row>
-    <row r="21" spans="6:22" x14ac:dyDescent="0.25">
+    <row r="21" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
       <c r="H21" s="6"/>
@@ -11798,7 +11908,7 @@
       <c r="U21" s="6"/>
       <c r="V21" s="6"/>
     </row>
-    <row r="22" spans="6:22" x14ac:dyDescent="0.25">
+    <row r="22" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F22" s="6"/>
       <c r="G22" s="6"/>
       <c r="H22" s="6"/>
@@ -11817,7 +11927,7 @@
       <c r="U22" s="6"/>
       <c r="V22" s="6"/>
     </row>
-    <row r="23" spans="6:22" x14ac:dyDescent="0.25">
+    <row r="23" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F23" s="6"/>
       <c r="G23" s="6"/>
       <c r="H23" s="6"/>
@@ -11836,7 +11946,7 @@
       <c r="U23" s="6"/>
       <c r="V23" s="6"/>
     </row>
-    <row r="24" spans="6:22" x14ac:dyDescent="0.25">
+    <row r="24" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
       <c r="H24" s="6"/>
@@ -11855,6 +11965,44 @@
       <c r="U24" s="6"/>
       <c r="V24" s="6"/>
     </row>
+    <row r="25" spans="6:24" x14ac:dyDescent="0.25">
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="6"/>
+      <c r="K25" s="6"/>
+      <c r="L25" s="6"/>
+      <c r="M25" s="6"/>
+      <c r="N25" s="6"/>
+      <c r="O25" s="6"/>
+      <c r="P25" s="6"/>
+      <c r="Q25" s="6"/>
+      <c r="R25" s="6"/>
+      <c r="S25" s="6"/>
+      <c r="T25" s="6"/>
+      <c r="U25" s="6"/>
+      <c r="V25" s="6"/>
+    </row>
+    <row r="26" spans="6:24" x14ac:dyDescent="0.25">
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="6"/>
+      <c r="K26" s="6"/>
+      <c r="L26" s="6"/>
+      <c r="M26" s="6"/>
+      <c r="N26" s="6"/>
+      <c r="O26" s="6"/>
+      <c r="P26" s="6"/>
+      <c r="Q26" s="6"/>
+      <c r="R26" s="6"/>
+      <c r="S26" s="6"/>
+      <c r="T26" s="6"/>
+      <c r="U26" s="6"/>
+      <c r="V26" s="6"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>